<commit_message>
macc e mauc prontas
</commit_message>
<xml_diff>
--- a/Python/combined_knn10.xlsx
+++ b/Python/combined_knn10.xlsx
@@ -8,19 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Rodrigo S. Hirama\Documentos\EACH\IC\Classification-of-mammography-images\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE25225-043E-49CB-9A37-B8E61CFB5625}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB555E6-5DE7-4A3A-8730-795383C93A5A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="combined" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>accuracy</t>
   </si>
@@ -38,6 +45,15 @@
   </si>
   <si>
     <t>0,05</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>std</t>
   </si>
 </sst>
 </file>
@@ -96,16 +112,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -168,12 +186,6 @@
               </a:rPr>
               <a:t>ε</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>  </a:t>
-            </a:r>
             <a:endParaRPr lang="pt-BR">
               <a:effectLst/>
             </a:endParaRPr>
@@ -225,7 +237,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.001</c:v>
+                  <c:v>0.10%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -322,7 +334,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-795F-4454-959C-0260EB4E1EBC}"/>
+              <c16:uniqueId val="{00000000-7659-464A-B23D-A00F50A8FE3F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -335,7 +347,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.01</c:v>
+                  <c:v>1%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -430,7 +442,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-795F-4454-959C-0260EB4E1EBC}"/>
+              <c16:uniqueId val="{00000001-7659-464A-B23D-A00F50A8FE3F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -443,7 +455,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.05</c:v>
+                  <c:v>5%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -540,7 +552,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-795F-4454-959C-0260EB4E1EBC}"/>
+              <c16:uniqueId val="{00000002-7659-464A-B23D-A00F50A8FE3F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -554,11 +566,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="157345392"/>
-        <c:axId val="81930432"/>
+        <c:axId val="524786223"/>
+        <c:axId val="783598655"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="157345392"/>
+        <c:axId val="524786223"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,11 +597,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
-                  <a:t>K-nearest</a:t>
+                  <a:t>K-Nearest</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="pt-BR" baseline="0"/>
-                  <a:t> neighbors</a:t>
+                  <a:t> Neighbors</a:t>
                 </a:r>
                 <a:endParaRPr lang="pt-BR"/>
               </a:p>
@@ -661,7 +673,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81930432"/>
+        <c:crossAx val="783598655"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -669,7 +681,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81930432"/>
+        <c:axId val="783598655"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -710,7 +722,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
-                  <a:t>Average accuracy</a:t>
+                  <a:t>Average Accuracy</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -775,7 +787,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157345392"/>
+        <c:crossAx val="524786223"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1375,23 +1387,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>149542</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>139064</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9771ACC7-5038-4F02-A0E7-FFA241CF30E2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C58BEAAC-6FCC-424B-8162-AFFA6C827209}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1678,10 +1690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE33"/>
+  <dimension ref="A1:AE38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K16" workbookViewId="0">
-      <selection activeCell="AJ32" sqref="AJ32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1780,42 +1792,42 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3" t="s">
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -4003,39 +4015,39 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="I30" s="4">
-        <v>1</v>
-      </c>
-      <c r="J30" s="4">
+      <c r="I30" s="3">
+        <v>1</v>
+      </c>
+      <c r="J30" s="3">
         <v>2</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K30" s="3">
         <v>3</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="3">
         <v>4</v>
       </c>
-      <c r="M30" s="4">
+      <c r="M30" s="3">
         <v>5</v>
       </c>
-      <c r="N30" s="4">
+      <c r="N30" s="3">
         <v>6</v>
       </c>
-      <c r="O30" s="4">
+      <c r="O30" s="3">
         <v>7</v>
       </c>
-      <c r="P30" s="4">
+      <c r="P30" s="3">
         <v>8</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="Q30" s="3">
         <v>9</v>
       </c>
-      <c r="R30" s="4">
+      <c r="R30" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="H31" s="4">
+      <c r="H31" s="5">
         <v>1E-3</v>
       </c>
       <c r="I31">
@@ -4070,7 +4082,7 @@
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="H32" s="4">
+      <c r="H32" s="6">
         <v>0.01</v>
       </c>
       <c r="I32">
@@ -4105,7 +4117,7 @@
       </c>
     </row>
     <row r="33" spans="8:18" x14ac:dyDescent="0.3">
-      <c r="H33" s="4">
+      <c r="H33" s="6">
         <v>0.05</v>
       </c>
       <c r="I33">
@@ -4137,6 +4149,68 @@
       </c>
       <c r="R33">
         <v>0.60360360360360366</v>
+      </c>
+    </row>
+    <row r="35" spans="8:18" x14ac:dyDescent="0.3">
+      <c r="I35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="8:18" x14ac:dyDescent="0.3">
+      <c r="H36" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="I36">
+        <f>MAX(I31:R31)</f>
+        <v>0.84684684684684686</v>
+      </c>
+      <c r="J36">
+        <f>AVERAGE(I31:R31)</f>
+        <v>0.81981981981981988</v>
+      </c>
+      <c r="K36">
+        <f>_xlfn.STDEV.S(I31:R31)</f>
+        <v>1.8018018018018007E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="8:18" x14ac:dyDescent="0.3">
+      <c r="H37" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="I37">
+        <f t="shared" ref="I37:I38" si="0">MAX(I32:R32)</f>
+        <v>0.83783783783783783</v>
+      </c>
+      <c r="J37">
+        <f t="shared" ref="J37:J38" si="1">AVERAGE(I32:R32)</f>
+        <v>0.80810810810810807</v>
+      </c>
+      <c r="K37">
+        <f t="shared" ref="K37:K38" si="2">_xlfn.STDEV.S(I32:R32)</f>
+        <v>1.8043025688648406E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="8:18" x14ac:dyDescent="0.3">
+      <c r="H38" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>0.69369369369369371</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>0.67567567567567566</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="2"/>
+        <v>2.7522977146881913E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4146,6 +4220,7 @@
     <mergeCell ref="V2:AE2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>